<commit_message>
Gantt-diagram updated with name of project
</commit_message>
<xml_diff>
--- a/doc/diagrams/Gantt/Gantt-diagram_kozosseg.xlsx
+++ b/doc/diagrams/Gantt/Gantt-diagram_kozosseg.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4FDE07-A087-421A-8B4A-A168440DDAC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2A7DC7-4CDF-4853-89F0-CD360EE7E60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,12 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
-    <t>Projekt neve</t>
-  </si>
-  <si>
-    <t>Gyakorlat ideje</t>
-  </si>
-  <si>
     <t>Projekt kezdete:</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
   </si>
   <si>
     <t>Mérföldkő II.</t>
-  </si>
-  <si>
-    <t>Mértföldkő III.</t>
   </si>
   <si>
     <t>Mérföldkő IIII.</t>
@@ -151,6 +142,15 @@
   </si>
   <si>
     <t>Madarász Máté</t>
+  </si>
+  <si>
+    <t>üzeneteSZTEk</t>
+  </si>
+  <si>
+    <t>Kedd 16:00</t>
+  </si>
+  <si>
+    <t>Mérföldkő III.</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1617,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1635,7 +1635,7 @@
     <row r="1" spans="1:84" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="23"/>
       <c r="B1" s="61" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="2" spans="1:84" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="27" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F2" s="40"/>
       <c r="H2" s="25"/>
@@ -1654,7 +1654,7 @@
     <row r="3" spans="1:84" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="27"/>
       <c r="C3" s="60" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="65">
         <v>44098</v>
@@ -1780,16 +1780,16 @@
     <row r="5" spans="1:84" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23"/>
       <c r="B5" s="54" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" s="67"/>
       <c r="H5" s="6">
@@ -2190,7 +2190,7 @@
     <row r="7" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="23"/>
       <c r="B7" s="56" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="11"/>
@@ -2281,10 +2281,10 @@
     <row r="8" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23"/>
       <c r="B8" s="46" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="28">
         <f>Project_Start</f>
@@ -2380,10 +2380,10 @@
     <row r="9" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23"/>
       <c r="B9" s="46" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D9" s="28">
         <f>Project_Start+8</f>
@@ -2479,7 +2479,7 @@
     <row r="10" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="23"/>
       <c r="B10" s="57" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="13"/>
@@ -2570,10 +2570,10 @@
     <row r="11" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="23"/>
       <c r="B11" s="52" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="29">
         <f>Project_Start+11</f>
@@ -2669,10 +2669,10 @@
     <row r="12" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="23"/>
       <c r="B12" s="52" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" s="29">
         <f>Project_Start+14</f>
@@ -2765,10 +2765,10 @@
     <row r="13" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="23"/>
       <c r="B13" s="52" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" s="29">
         <f>Project_Start+14</f>
@@ -2861,10 +2861,10 @@
     <row r="14" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="23"/>
       <c r="B14" s="52" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" s="53" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" s="29">
         <f>Project_Start+11</f>
@@ -2957,10 +2957,10 @@
     <row r="15" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="23"/>
       <c r="B15" s="52" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D15" s="29">
         <f>Project_Start+18</f>
@@ -3053,10 +3053,10 @@
     <row r="16" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="23"/>
       <c r="B16" s="52" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D16" s="29">
         <f>Project_Start+18</f>
@@ -3149,10 +3149,10 @@
     <row r="17" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="23"/>
       <c r="B17" s="52" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" s="29">
         <f>Project_Start+23</f>
@@ -3245,7 +3245,7 @@
     <row r="18" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="23"/>
       <c r="B18" s="58" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="15"/>
@@ -3338,10 +3338,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D19" s="30">
         <f>Project_Start+25</f>
@@ -3437,10 +3437,10 @@
     <row r="20" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="23"/>
       <c r="B20" s="50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D20" s="30">
         <f>Project_Start+25</f>
@@ -3533,10 +3533,10 @@
     <row r="21" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="23"/>
       <c r="B21" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="51" t="s">
         <v>28</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>31</v>
       </c>
       <c r="D21" s="30">
         <f>Project_Start+32</f>
@@ -3629,10 +3629,10 @@
     <row r="22" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="23"/>
       <c r="B22" s="50" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D22" s="30">
         <f>Project_Start+32</f>
@@ -3725,10 +3725,10 @@
     <row r="23" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="23"/>
       <c r="B23" s="50" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D23" s="30">
         <f>Project_Start+37</f>
@@ -3821,7 +3821,7 @@
     <row r="24" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="23"/>
       <c r="B24" s="59" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C24" s="35"/>
       <c r="D24" s="17"/>
@@ -3912,10 +3912,10 @@
     <row r="25" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="23"/>
       <c r="B25" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="49" t="s">
         <v>33</v>
-      </c>
-      <c r="C25" s="49" t="s">
-        <v>36</v>
       </c>
       <c r="D25" s="31">
         <f>Project_Start+39</f>
@@ -4011,10 +4011,10 @@
     <row r="26" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="23"/>
       <c r="B26" s="48" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D26" s="31">
         <f>Project_Start+46</f>
@@ -4107,10 +4107,10 @@
     <row r="27" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="23"/>
       <c r="B27" s="48" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D27" s="31">
         <f>Project_Start+46</f>
@@ -4203,10 +4203,10 @@
     <row r="28" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="23"/>
       <c r="B28" s="48" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D28" s="31">
         <f>Project_Start+64</f>
@@ -4394,6 +4394,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="BS4:BY4"/>
+    <mergeCell ref="BZ4:CF4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="D3:E3"/>
@@ -4402,11 +4407,6 @@
     <mergeCell ref="V4:AB4"/>
     <mergeCell ref="AC4:AI4"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="BL4:BR4"/>
-    <mergeCell ref="BS4:BY4"/>
-    <mergeCell ref="BZ4:CF4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BX9 BZ6:CE9 H29:BX29 BZ29:CE29">
     <cfRule type="expression" dxfId="41" priority="88">

</xml_diff>

<commit_message>
updated Gantt-diagram with new tasks of IV. milestone
</commit_message>
<xml_diff>
--- a/doc/diagrams/Gantt/Gantt-diagram_kozosseg.xlsx
+++ b/doc/diagrams/Gantt/Gantt-diagram_kozosseg.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2A7DC7-4CDF-4853-89F0-CD360EE7E60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5C6172-AEF3-4603-A909-FAE6A18DC754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1013" yWindow="1312" windowWidth="21022" windowHeight="13088" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Projekt kezdete:</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>Mérföldkő III.</t>
+  </si>
+  <si>
+    <t>JUnit tesztkörnyezet előkészítése</t>
+  </si>
+  <si>
+    <t>SEO optimalizálás</t>
+  </si>
+  <si>
+    <t>Projekt optimalizálás (képek, kód tömörítése stb..)</t>
   </si>
 </sst>
 </file>
@@ -1613,17 +1622,17 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CF32"/>
+  <dimension ref="A1:CF35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="22" customWidth="1"/>
-    <col min="2" max="2" width="36.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.06640625" customWidth="1"/>
     <col min="4" max="4" width="10.3984375" style="4" customWidth="1"/>
     <col min="5" max="5" width="10.3984375" customWidth="1"/>
@@ -2197,7 +2206,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="37"/>
       <c r="G7" s="10" t="str">
-        <f t="shared" ref="G7:G29" si="23">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G7:G32" si="23">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H7" s="38"/>
@@ -4021,8 +4030,8 @@
         <v>44144</v>
       </c>
       <c r="E26" s="31">
-        <f>Project_Start+63</f>
-        <v>44161</v>
+        <f>Project_Start+53</f>
+        <v>44151</v>
       </c>
       <c r="F26" s="37"/>
       <c r="G26" s="10"/>
@@ -4107,18 +4116,18 @@
     <row r="27" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="23"/>
       <c r="B27" s="48" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C27" s="49" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="31">
-        <f>Project_Start+46</f>
-        <v>44144</v>
+        <f>Project_Start+54</f>
+        <v>44152</v>
       </c>
       <c r="E27" s="31">
-        <f>Project_Start+63</f>
-        <v>44161</v>
+        <f>Project_Start+57</f>
+        <v>44155</v>
       </c>
       <c r="F27" s="37"/>
       <c r="G27" s="10"/>
@@ -4203,18 +4212,18 @@
     <row r="28" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="23"/>
       <c r="B28" s="48" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D28" s="31">
-        <f>Project_Start+64</f>
-        <v>44162</v>
+        <f>Project_Start+58</f>
+        <v>44156</v>
       </c>
       <c r="E28" s="31">
-        <f>Project_Start+66</f>
-        <v>44164</v>
+        <f>Project_Start+63</f>
+        <v>44161</v>
       </c>
       <c r="F28" s="37"/>
       <c r="G28" s="10"/>
@@ -4298,15 +4307,22 @@
     </row>
     <row r="29" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="23"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
+      <c r="B29" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="31">
+        <f>Project_Start+46</f>
+        <v>44144</v>
+      </c>
+      <c r="E29" s="31">
+        <f>Project_Start+55</f>
+        <v>44153</v>
+      </c>
       <c r="F29" s="37"/>
-      <c r="G29" s="19" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
+      <c r="G29" s="10"/>
       <c r="H29" s="38"/>
       <c r="I29" s="38"/>
       <c r="J29" s="38"/>
@@ -4385,20 +4401,296 @@
       <c r="CE29" s="38"/>
       <c r="CF29" s="38"/>
     </row>
-    <row r="31" spans="1:84" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C31" s="8"/>
-      <c r="E31" s="24"/>
+    <row r="30" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="23"/>
+      <c r="B30" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="31">
+        <f>Project_Start+56</f>
+        <v>44154</v>
+      </c>
+      <c r="E30" s="31">
+        <f>Project_Start+63</f>
+        <v>44161</v>
+      </c>
+      <c r="F30" s="37"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="38"/>
+      <c r="U30" s="38"/>
+      <c r="V30" s="38"/>
+      <c r="W30" s="38"/>
+      <c r="X30" s="38"/>
+      <c r="Y30" s="38"/>
+      <c r="Z30" s="38"/>
+      <c r="AA30" s="38"/>
+      <c r="AB30" s="38"/>
+      <c r="AC30" s="38"/>
+      <c r="AD30" s="38"/>
+      <c r="AE30" s="38"/>
+      <c r="AF30" s="38"/>
+      <c r="AG30" s="38"/>
+      <c r="AH30" s="38"/>
+      <c r="AI30" s="38"/>
+      <c r="AJ30" s="38"/>
+      <c r="AK30" s="38"/>
+      <c r="AL30" s="38"/>
+      <c r="AM30" s="38"/>
+      <c r="AN30" s="38"/>
+      <c r="AO30" s="38"/>
+      <c r="AP30" s="38"/>
+      <c r="AQ30" s="38"/>
+      <c r="AR30" s="38"/>
+      <c r="AS30" s="38"/>
+      <c r="AT30" s="38"/>
+      <c r="AU30" s="38"/>
+      <c r="AV30" s="38"/>
+      <c r="AW30" s="38"/>
+      <c r="AX30" s="38"/>
+      <c r="AY30" s="38"/>
+      <c r="AZ30" s="38"/>
+      <c r="BA30" s="38"/>
+      <c r="BB30" s="38"/>
+      <c r="BC30" s="38"/>
+      <c r="BD30" s="38"/>
+      <c r="BE30" s="38"/>
+      <c r="BF30" s="38"/>
+      <c r="BG30" s="38"/>
+      <c r="BH30" s="38"/>
+      <c r="BI30" s="38"/>
+      <c r="BJ30" s="38"/>
+      <c r="BK30" s="38"/>
+      <c r="BL30" s="38"/>
+      <c r="BM30" s="38"/>
+      <c r="BN30" s="38"/>
+      <c r="BO30" s="38"/>
+      <c r="BP30" s="38"/>
+      <c r="BQ30" s="38"/>
+      <c r="BR30" s="38"/>
+      <c r="BS30" s="38"/>
+      <c r="BT30" s="38"/>
+      <c r="BU30" s="38"/>
+      <c r="BV30" s="38"/>
+      <c r="BW30" s="38"/>
+      <c r="BX30" s="38"/>
+      <c r="BY30" s="38"/>
+      <c r="BZ30" s="38"/>
+      <c r="CA30" s="38"/>
+      <c r="CB30" s="38"/>
+      <c r="CC30" s="38"/>
+      <c r="CD30" s="38"/>
+      <c r="CE30" s="38"/>
+      <c r="CF30" s="38"/>
     </row>
-    <row r="32" spans="1:84" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C32" s="9"/>
+    <row r="31" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="23"/>
+      <c r="B31" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="31">
+        <f>Project_Start+64</f>
+        <v>44162</v>
+      </c>
+      <c r="E31" s="31">
+        <f>Project_Start+66</f>
+        <v>44164</v>
+      </c>
+      <c r="F31" s="37"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
+      <c r="R31" s="38"/>
+      <c r="S31" s="38"/>
+      <c r="T31" s="38"/>
+      <c r="U31" s="38"/>
+      <c r="V31" s="38"/>
+      <c r="W31" s="38"/>
+      <c r="X31" s="38"/>
+      <c r="Y31" s="38"/>
+      <c r="Z31" s="38"/>
+      <c r="AA31" s="38"/>
+      <c r="AB31" s="38"/>
+      <c r="AC31" s="38"/>
+      <c r="AD31" s="38"/>
+      <c r="AE31" s="38"/>
+      <c r="AF31" s="38"/>
+      <c r="AG31" s="38"/>
+      <c r="AH31" s="38"/>
+      <c r="AI31" s="38"/>
+      <c r="AJ31" s="38"/>
+      <c r="AK31" s="38"/>
+      <c r="AL31" s="38"/>
+      <c r="AM31" s="38"/>
+      <c r="AN31" s="38"/>
+      <c r="AO31" s="38"/>
+      <c r="AP31" s="38"/>
+      <c r="AQ31" s="38"/>
+      <c r="AR31" s="38"/>
+      <c r="AS31" s="38"/>
+      <c r="AT31" s="38"/>
+      <c r="AU31" s="38"/>
+      <c r="AV31" s="38"/>
+      <c r="AW31" s="38"/>
+      <c r="AX31" s="38"/>
+      <c r="AY31" s="38"/>
+      <c r="AZ31" s="38"/>
+      <c r="BA31" s="38"/>
+      <c r="BB31" s="38"/>
+      <c r="BC31" s="38"/>
+      <c r="BD31" s="38"/>
+      <c r="BE31" s="38"/>
+      <c r="BF31" s="38"/>
+      <c r="BG31" s="38"/>
+      <c r="BH31" s="38"/>
+      <c r="BI31" s="38"/>
+      <c r="BJ31" s="38"/>
+      <c r="BK31" s="38"/>
+      <c r="BL31" s="38"/>
+      <c r="BM31" s="38"/>
+      <c r="BN31" s="38"/>
+      <c r="BO31" s="38"/>
+      <c r="BP31" s="38"/>
+      <c r="BQ31" s="38"/>
+      <c r="BR31" s="38"/>
+      <c r="BS31" s="38"/>
+      <c r="BT31" s="38"/>
+      <c r="BU31" s="38"/>
+      <c r="BV31" s="38"/>
+      <c r="BW31" s="38"/>
+      <c r="BX31" s="38"/>
+      <c r="BY31" s="38"/>
+      <c r="BZ31" s="38"/>
+      <c r="CA31" s="38"/>
+      <c r="CB31" s="38"/>
+      <c r="CC31" s="38"/>
+      <c r="CD31" s="38"/>
+      <c r="CE31" s="38"/>
+      <c r="CF31" s="38"/>
+    </row>
+    <row r="32" spans="1:84" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A32" s="23"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="19" t="str">
+        <f t="shared" si="23"/>
+        <v/>
+      </c>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="38"/>
+      <c r="S32" s="38"/>
+      <c r="T32" s="38"/>
+      <c r="U32" s="38"/>
+      <c r="V32" s="38"/>
+      <c r="W32" s="38"/>
+      <c r="X32" s="38"/>
+      <c r="Y32" s="38"/>
+      <c r="Z32" s="38"/>
+      <c r="AA32" s="38"/>
+      <c r="AB32" s="38"/>
+      <c r="AC32" s="38"/>
+      <c r="AD32" s="38"/>
+      <c r="AE32" s="38"/>
+      <c r="AF32" s="38"/>
+      <c r="AG32" s="38"/>
+      <c r="AH32" s="38"/>
+      <c r="AI32" s="38"/>
+      <c r="AJ32" s="38"/>
+      <c r="AK32" s="38"/>
+      <c r="AL32" s="38"/>
+      <c r="AM32" s="38"/>
+      <c r="AN32" s="38"/>
+      <c r="AO32" s="38"/>
+      <c r="AP32" s="38"/>
+      <c r="AQ32" s="38"/>
+      <c r="AR32" s="38"/>
+      <c r="AS32" s="38"/>
+      <c r="AT32" s="38"/>
+      <c r="AU32" s="38"/>
+      <c r="AV32" s="38"/>
+      <c r="AW32" s="38"/>
+      <c r="AX32" s="38"/>
+      <c r="AY32" s="38"/>
+      <c r="AZ32" s="38"/>
+      <c r="BA32" s="38"/>
+      <c r="BB32" s="38"/>
+      <c r="BC32" s="38"/>
+      <c r="BD32" s="38"/>
+      <c r="BE32" s="38"/>
+      <c r="BF32" s="38"/>
+      <c r="BG32" s="38"/>
+      <c r="BH32" s="38"/>
+      <c r="BI32" s="38"/>
+      <c r="BJ32" s="38"/>
+      <c r="BK32" s="38"/>
+      <c r="BL32" s="38"/>
+      <c r="BM32" s="38"/>
+      <c r="BN32" s="38"/>
+      <c r="BO32" s="38"/>
+      <c r="BP32" s="38"/>
+      <c r="BQ32" s="38"/>
+      <c r="BR32" s="38"/>
+      <c r="BS32" s="38"/>
+      <c r="BT32" s="38"/>
+      <c r="BU32" s="38"/>
+      <c r="BV32" s="38"/>
+      <c r="BW32" s="38"/>
+      <c r="BX32" s="38"/>
+      <c r="BY32" s="38"/>
+      <c r="BZ32" s="38"/>
+      <c r="CA32" s="38"/>
+      <c r="CB32" s="38"/>
+      <c r="CC32" s="38"/>
+      <c r="CD32" s="38"/>
+      <c r="CE32" s="38"/>
+      <c r="CF32" s="38"/>
+    </row>
+    <row r="34" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C34" s="8"/>
+      <c r="E34" s="24"/>
+    </row>
+    <row r="35" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="BL4:BR4"/>
-    <mergeCell ref="BS4:BY4"/>
-    <mergeCell ref="BZ4:CF4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="D3:E3"/>
@@ -4407,13 +4699,18 @@
     <mergeCell ref="V4:AB4"/>
     <mergeCell ref="AC4:AI4"/>
     <mergeCell ref="F4:F5"/>
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="BS4:BY4"/>
+    <mergeCell ref="BZ4:CF4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BX9 BZ6:CE9 H29:BX29 BZ29:CE29">
+  <conditionalFormatting sqref="H5:BX9 BZ6:CE9 H32:BX32 BZ32:CE32">
     <cfRule type="expression" dxfId="41" priority="88">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:BX9 BZ6:CE9 H29:BX29 BZ29:CE29">
+  <conditionalFormatting sqref="H6:BX9 BZ6:CE9 H32:BX32 BZ32:CE32">
     <cfRule type="expression" dxfId="40" priority="82">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -4421,12 +4718,12 @@
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BZ5:CF5 BY5:BY9 CF6:CF9 BY29 CF29">
+  <conditionalFormatting sqref="BZ5:CF5 BY5:BY9 CF6:CF9 BY32 CF32">
     <cfRule type="expression" dxfId="38" priority="90">
       <formula>AND(TODAY()&gt;=BY$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BY6:BY9 CF6:CF9 BY29 CF29">
+  <conditionalFormatting sqref="BY6:BY9 CF6:CF9 BY32 CF32">
     <cfRule type="expression" dxfId="37" priority="93">
       <formula>AND(task_start&lt;=BY$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BY$5)</formula>
     </cfRule>
@@ -4564,12 +4861,12 @@
       <formula>AND(task_end&gt;=BY$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25:BX28 BZ25:CE28">
+  <conditionalFormatting sqref="H25:BX31 BZ25:CE31">
     <cfRule type="expression" dxfId="5" priority="9">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25:BX28 BZ25:CE28">
+  <conditionalFormatting sqref="H25:BX31 BZ25:CE31">
     <cfRule type="expression" dxfId="4" priority="7">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -4577,12 +4874,12 @@
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BY25:BY28 CF25:CF28">
+  <conditionalFormatting sqref="BY25:BY31 CF25:CF31">
     <cfRule type="expression" dxfId="2" priority="10">
       <formula>AND(TODAY()&gt;=BY$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BY25:BY28 CF25:CF28">
+  <conditionalFormatting sqref="BY25:BY31 CF25:CF31">
     <cfRule type="expression" dxfId="1" priority="11">
       <formula>AND(task_start&lt;=BY$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BY$5)</formula>
     </cfRule>

</xml_diff>